<commit_message>
Nộp bài tập Python
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>STT</t>
   </si>
@@ -37,28 +37,19 @@
     <t>Coca</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>15000</t>
-  </si>
-  <si>
     <t>SP2</t>
   </si>
   <si>
     <t>Pepsi</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>18000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -96,9 +87,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +420,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -432,28 +429,28 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="D2" s="2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3">
+        <v>18000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>